<commit_message>
Atualização do estudo final
Criação de mais coluna na planilha
</commit_message>
<xml_diff>
--- a/SAF_Estudo final.xlsx
+++ b/SAF_Estudo final.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\igorc\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\igorc\Documents\GitProjetos\AGROFV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFF87F45-3AF2-426A-94BB-C80F5ACC9A8A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42FA069B-72A7-47BB-A1FE-0F833018FE51}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7125" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -84,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="33">
   <si>
     <t>Dia_Juliano</t>
   </si>
@@ -271,12 +271,21 @@
   <si>
     <t>Fator de capacidade (%)</t>
   </si>
+  <si>
+    <t>Dias com interrupções</t>
+  </si>
+  <si>
+    <t>Dias sem interrupções</t>
+  </si>
+  <si>
+    <t>Dias sem geração</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -303,6 +312,13 @@
     <font>
       <b/>
       <vertAlign val="superscript"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -354,10 +370,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -380,10 +397,13 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Porcentagem" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -7267,51 +7287,63 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00DE381F-A64E-4A77-B761-4733C6AC8E04}">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.85546875" customWidth="1"/>
-    <col min="3" max="3" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="24.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="27.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="17" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="10">
+      <c r="I1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="11">
         <v>44835</v>
       </c>
       <c r="B2" s="2">
@@ -7326,7 +7358,7 @@
         <v>9882.6</v>
       </c>
       <c r="E2" s="2">
-        <f>D2/$B$21</f>
+        <f t="shared" ref="E2:E8" si="0">D2/$B$21</f>
         <v>140.47761194029849</v>
       </c>
       <c r="F2" s="2">
@@ -7337,13 +7369,22 @@
         <f>D2/($B$21*(24*31))</f>
         <v>0.18881399454341194</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="16">
         <f>E2/F2</f>
         <v>0.76743772821013623</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="10">
+      <c r="I2">
+        <v>9</v>
+      </c>
+      <c r="J2">
+        <v>21</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="11">
         <v>44866</v>
       </c>
       <c r="B3" s="2">
@@ -7351,31 +7392,40 @@
         <v>171.43549084923526</v>
       </c>
       <c r="C3" s="2">
-        <f t="shared" ref="C3:C13" si="0">B3*$B$20</f>
+        <f t="shared" ref="C3:C13" si="1">B3*$B$20</f>
         <v>63709.78423252733</v>
       </c>
       <c r="D3">
         <v>9481</v>
       </c>
       <c r="E3" s="2">
-        <f>D3/$B$21</f>
+        <f t="shared" si="0"/>
         <v>134.7690120824449</v>
       </c>
       <c r="F3" s="2">
-        <f t="shared" ref="F3:F13" si="1">B3/1</f>
+        <f t="shared" ref="F3:F13" si="2">B3/1</f>
         <v>171.43549084923526</v>
       </c>
       <c r="G3" s="16">
         <f>D3/($B$21*(24*30))</f>
         <v>0.18717918344784013</v>
       </c>
-      <c r="H3">
-        <f t="shared" ref="H3:H13" si="2">E3/F3</f>
+      <c r="H3" s="16">
+        <f t="shared" ref="H3:H13" si="3">E3/F3</f>
         <v>0.78612084005968286</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="10">
+      <c r="I3">
+        <v>17</v>
+      </c>
+      <c r="J3">
+        <v>14</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="11">
         <v>44896</v>
       </c>
       <c r="B4" s="2">
@@ -7383,31 +7433,40 @@
         <v>188.82980785481257</v>
       </c>
       <c r="C4" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>70173.954386606332</v>
       </c>
       <c r="D4">
         <v>10187.9</v>
       </c>
       <c r="E4" s="2">
-        <f>D4/$B$21</f>
+        <f t="shared" si="0"/>
         <v>144.81734186211796</v>
       </c>
       <c r="F4" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>188.82980785481257</v>
       </c>
       <c r="G4" s="16">
-        <f t="shared" ref="G3:G13" si="3">D4/($B$21*(24*31))</f>
+        <f t="shared" ref="G4:G11" si="4">D4/($B$21*(24*31))</f>
         <v>0.1946469648684381</v>
       </c>
-      <c r="H4">
-        <f t="shared" si="2"/>
+      <c r="H4" s="16">
+        <f t="shared" si="3"/>
         <v>0.76691992385791696</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="10">
+      <c r="I4">
+        <v>14</v>
+      </c>
+      <c r="J4">
+        <v>16</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="11">
         <v>44927</v>
       </c>
       <c r="B5" s="2">
@@ -7415,31 +7474,40 @@
         <v>186.30746214999982</v>
       </c>
       <c r="C5" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>69236.586634938256</v>
       </c>
       <c r="D5">
         <v>8744.5</v>
       </c>
       <c r="E5" s="2">
-        <f>D5/$B$21</f>
+        <f t="shared" si="0"/>
         <v>124.29992892679458</v>
       </c>
       <c r="F5" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>186.30746214999982</v>
       </c>
       <c r="G5" s="16">
+        <f t="shared" si="4"/>
+        <v>0.16706979694461638</v>
+      </c>
+      <c r="H5" s="16">
         <f t="shared" si="3"/>
-        <v>0.16706979694461638</v>
-      </c>
-      <c r="H5">
-        <f t="shared" si="2"/>
         <v>0.66717633041836111</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="10">
+      <c r="I5">
+        <v>17</v>
+      </c>
+      <c r="J5">
+        <v>13</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="11">
         <v>44958</v>
       </c>
       <c r="B6" s="2">
@@ -7447,31 +7515,40 @@
         <v>150.25488893333323</v>
       </c>
       <c r="C6" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>55838.534403844656</v>
       </c>
       <c r="D6">
         <v>8055.5</v>
       </c>
       <c r="E6" s="2">
-        <f>D6/$B$21</f>
+        <f t="shared" si="0"/>
         <v>114.50604122245912</v>
       </c>
       <c r="F6" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>150.25488893333323</v>
       </c>
       <c r="G6" s="16">
         <f>D6/($B$21*(24*28))</f>
         <v>0.17039589467627844</v>
       </c>
-      <c r="H6">
-        <f t="shared" si="2"/>
+      <c r="H6" s="16">
+        <f t="shared" si="3"/>
         <v>0.76207863874076298</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="10">
+      <c r="I6">
+        <v>12</v>
+      </c>
+      <c r="J6">
+        <v>15</v>
+      </c>
+      <c r="K6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="11">
         <v>44986</v>
       </c>
       <c r="B7" s="2">
@@ -7479,31 +7556,40 @@
         <v>161.74506135833323</v>
       </c>
       <c r="C7" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>60108.574419275632</v>
       </c>
       <c r="D7">
         <v>9001.5</v>
       </c>
       <c r="E7" s="2">
-        <f>D7/$B$21</f>
+        <f t="shared" si="0"/>
         <v>127.95309168443495</v>
       </c>
       <c r="F7" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>161.74506135833323</v>
       </c>
       <c r="G7" s="16">
         <f>D7/($B$21*(24*31))</f>
         <v>0.17197996194144483</v>
       </c>
-      <c r="H7">
-        <f t="shared" si="2"/>
+      <c r="H7" s="16">
+        <f t="shared" si="3"/>
         <v>0.79107881631677845</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="10">
+      <c r="I7">
+        <v>19</v>
+      </c>
+      <c r="J7">
+        <v>9</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="11">
         <v>45017</v>
       </c>
       <c r="B8" s="2">
@@ -7511,31 +7597,40 @@
         <v>154.26365726666654</v>
       </c>
       <c r="C8" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>57328.294571297127</v>
       </c>
       <c r="D8">
         <v>7356</v>
       </c>
       <c r="E8" s="2">
-        <f>D8/$B$21</f>
+        <f t="shared" si="0"/>
         <v>104.56289978678038</v>
       </c>
       <c r="F8" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>154.26365726666654</v>
       </c>
       <c r="G8" s="16">
         <f>D8/($B$21*(24*30))</f>
         <v>0.14522624970386161</v>
       </c>
-      <c r="H8">
-        <f t="shared" si="2"/>
+      <c r="H8" s="16">
+        <f t="shared" si="3"/>
         <v>0.67781940114403372</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="10">
+      <c r="I8">
+        <v>14</v>
+      </c>
+      <c r="J8">
+        <v>17</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="11">
         <v>45047</v>
       </c>
       <c r="B9" s="2">
@@ -7543,31 +7638,40 @@
         <v>146.36008349166653</v>
       </c>
       <c r="C9" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>54391.125742504642</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>1546.8</v>
       </c>
       <c r="E9" s="2">
-        <f t="shared" ref="E9:E13" si="4">D9/$B$21</f>
-        <v>0</v>
+        <f t="shared" ref="E9:E13" si="5">D9/$B$21</f>
+        <v>21.987206823027716</v>
       </c>
       <c r="F9" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>146.36008349166653</v>
       </c>
       <c r="G9" s="16">
         <f>D9/($B$21*(24*31))</f>
+        <v>2.9552697342779186E-2</v>
+      </c>
+      <c r="H9" s="16">
+        <f t="shared" si="3"/>
+        <v>0.15022679885448156</v>
+      </c>
+      <c r="I9">
         <v>0</v>
       </c>
-      <c r="H9">
-        <f t="shared" si="2"/>
+      <c r="J9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="10">
+      <c r="K9">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="11">
         <v>45078</v>
       </c>
       <c r="B10" s="2">
@@ -7575,31 +7679,40 @@
         <v>119.29126767499992</v>
       </c>
       <c r="C10" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>44331.66602055906</v>
       </c>
       <c r="D10">
         <v>6452.4</v>
       </c>
       <c r="E10" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>91.718550106609797</v>
       </c>
       <c r="F10" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>119.29126767499992</v>
       </c>
       <c r="G10" s="16">
         <f>D10/($B$21*(24*30))</f>
         <v>0.12738687514806915</v>
       </c>
-      <c r="H10">
-        <f t="shared" si="2"/>
+      <c r="H10" s="16">
+        <f t="shared" si="3"/>
         <v>0.76886223018846678</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="10">
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>6</v>
+      </c>
+      <c r="K10">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="11">
         <v>45108</v>
       </c>
       <c r="B11" s="2">
@@ -7607,31 +7720,40 @@
         <v>137.0277508499999</v>
       </c>
       <c r="C11" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>50922.993816953567</v>
       </c>
       <c r="D11">
         <v>8162.1</v>
       </c>
       <c r="E11" s="2">
+        <f t="shared" si="5"/>
+        <v>116.02132196162046</v>
+      </c>
+      <c r="F11" s="2">
+        <f t="shared" si="2"/>
+        <v>137.0277508499999</v>
+      </c>
+      <c r="G11" s="16">
         <f t="shared" si="4"/>
-        <v>116.02132196162046</v>
-      </c>
-      <c r="F11" s="2">
-        <f t="shared" si="1"/>
-        <v>137.0277508499999</v>
-      </c>
-      <c r="G11" s="16">
+        <v>0.15594263704518879</v>
+      </c>
+      <c r="H11" s="16">
         <f t="shared" si="3"/>
-        <v>0.15594263704518879</v>
-      </c>
-      <c r="H11">
-        <f t="shared" si="2"/>
         <v>0.84669945497846966</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="10">
+      <c r="I11">
+        <v>3</v>
+      </c>
+      <c r="J11">
+        <v>27</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="11">
         <v>45139</v>
       </c>
       <c r="B12" s="2">
@@ -7639,31 +7761,31 @@
         <v>155.30792533333326</v>
       </c>
       <c r="C12" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>57716.371117633513</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>8753.9</v>
       </c>
       <c r="E12" s="2">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>124.43354655294952</v>
       </c>
       <c r="F12" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>155.30792533333326</v>
       </c>
       <c r="G12" s="16">
         <f>D12/($B$21*(24*31))</f>
-        <v>0</v>
-      </c>
-      <c r="H12">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="10">
+        <v>0.16724939052815796</v>
+      </c>
+      <c r="H12" s="16">
+        <f t="shared" si="3"/>
+        <v>0.80120538785049844</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="11">
         <v>45170</v>
       </c>
       <c r="B13" s="2">
@@ -7671,33 +7793,33 @@
         <v>152.29600091666654</v>
       </c>
       <c r="C13" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>56597.063477424585</v>
       </c>
       <c r="D13">
         <v>4825</v>
       </c>
       <c r="E13" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>68.58564321250887</v>
       </c>
       <c r="F13" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>152.29600091666654</v>
       </c>
       <c r="G13" s="16">
         <f>D13/($B$21*(24*30))</f>
         <v>9.5257837795151221E-2</v>
       </c>
-      <c r="H13">
-        <f t="shared" si="2"/>
+      <c r="H13" s="16">
+        <f t="shared" si="3"/>
         <v>0.45034434784691174</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="10"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
         <v>25</v>
       </c>
@@ -7710,7 +7832,7 @@
       </c>
       <c r="D15" s="15"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
         <v>19</v>
       </c>

</xml_diff>

<commit_message>
implementação do executável 3
</commit_message>
<xml_diff>
--- a/SAF_Estudo final.xlsx
+++ b/SAF_Estudo final.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20416"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\igorc\Documents\GitProjetos\AGROFV\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\i5\Documents\GitProjetos\AGROFV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42FA069B-72A7-47BB-A1FE-0F833018FE51}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7125" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7125"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="5" r:id="rId1"/>
@@ -24,7 +23,7 @@
     <definedName name="somas_irradiacao_dia_juliano_1" localSheetId="2">'2023'!$A$64:$C$150</definedName>
     <definedName name="somas_irradiacao_dia_juliano_2" localSheetId="2">'2023'!$A$155:$C$293</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,8 +33,8 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
-  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" name="somas_irradiacao_dia_juliano" type="6" refreshedVersion="5" background="1" saveData="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <connection id="1" name="somas_irradiacao_dia_juliano" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="850" sourceFile="C:\Users\i5\Documents\GitProjetos\AGROFV\somas_irradiacao_dia_juliano.csv" comma="1">
       <textFields count="3">
         <textField/>
@@ -44,7 +43,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="2" xr16:uid="{00000000-0015-0000-FFFF-FFFF01000000}" name="somas_irradiacao_dia_juliano_11" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="2" name="somas_irradiacao_dia_juliano_11" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="850" firstRow="2" sourceFile="C:\Users\i5\Documents\GitProjetos\AGROFV\somas_irradiacao_dia_juliano_1.csv" comma="1">
       <textFields count="3">
         <textField/>
@@ -53,7 +52,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="3" xr16:uid="{00000000-0015-0000-FFFF-FFFF02000000}" name="somas_irradiacao_dia_juliano11" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="3" name="somas_irradiacao_dia_juliano11" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="850" sourceFile="C:\Users\i5\Documents\GitProjetos\AGROFV\somas_irradiacao_dia_juliano.csv" comma="1">
       <textFields count="3">
         <textField/>
@@ -62,7 +61,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="4" xr16:uid="{00000000-0015-0000-FFFF-FFFF03000000}" name="somas_irradiacao_dia_juliano21" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="4" name="somas_irradiacao_dia_juliano21" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="850" firstRow="2" sourceFile="C:\Users\i5\Documents\GitProjetos\AGROFV\somas_irradiacao_dia_juliano.csv" comma="1">
       <textFields count="3">
         <textField/>
@@ -71,7 +70,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="5" xr16:uid="{00000000-0015-0000-FFFF-FFFF04000000}" name="somas_irradiacao_dia_juliano3" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="5" name="somas_irradiacao_dia_juliano3" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="850" firstRow="2" sourceFile="C:\Users\i5\Documents\GitProjetos\AGROFV\somas_irradiacao_dia_juliano.csv" comma="1">
       <textFields count="3">
         <textField/>
@@ -284,7 +283,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -374,7 +373,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -394,12 +393,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -419,7 +419,579 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Planilha1!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Energia gerada (kWh)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Planilha1!$D$2:$D$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>9882.6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9481</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10187.9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8744.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8055.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9001.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7356</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1546.8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6452.4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8162.1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8753.9</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4825</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="-1501961056"/>
+        <c:axId val="-1501967584"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-1501961056"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1501967584"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-1501967584"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1501961056"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Planilha1!$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>PR (%)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Planilha1!$H$2:$H$13</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.76743772821013623</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.78612084005968286</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.76691992385791696</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.66717633041836111</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.76207863874076298</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.79107881631677845</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.67781940114403372</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.15022679885448156</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.76886223018846678</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.84669945497846966</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.80120538785049844</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.45034434784691174</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="-1501956160"/>
+        <c:axId val="-1501959968"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-1501956160"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1501959968"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-1501959968"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1501956160"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="pt-BR"/>
   <c:roundedCorners val="0"/>
@@ -797,7 +1369,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-8CAD-45ED-BF64-95483207E91A}"/>
             </c:ext>
@@ -1098,7 +1670,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-8CAD-45ED-BF64-95483207E91A}"/>
             </c:ext>
@@ -1127,11 +1699,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:smooth val="0"/>
-        <c:axId val="144858432"/>
-        <c:axId val="144853152"/>
+        <c:axId val="-1501957248"/>
+        <c:axId val="-1501966496"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="144858432"/>
+        <c:axId val="-1501957248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1228,7 +1800,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="144853152"/>
+        <c:crossAx val="-1501966496"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1236,7 +1808,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="144853152"/>
+        <c:axId val="-1501966496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="2.5"/>
@@ -1351,7 +1923,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="144858432"/>
+        <c:crossAx val="-1501957248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1365,14 +1937,14 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1407,8 +1979,8 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="pt-BR"/>
   <c:roundedCorners val="0"/>
@@ -2020,7 +2592,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-7652-4CDE-A25B-FC495EBA1889}"/>
             </c:ext>
@@ -2034,11 +2606,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="677534496"/>
-        <c:axId val="677542656"/>
+        <c:axId val="-1501963232"/>
+        <c:axId val="-1501961600"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="677534496"/>
+        <c:axId val="-1501963232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="2"/>
@@ -2096,12 +2668,12 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="677542656"/>
+        <c:crossAx val="-1501961600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="677542656"/>
+        <c:axId val="-1501961600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="2"/>
@@ -2159,7 +2731,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="677534496"/>
+        <c:crossAx val="-1501963232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2173,14 +2745,14 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -2215,8 +2787,8 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="pt-BR"/>
   <c:roundedCorners val="0"/>
@@ -2400,7 +2972,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-FC38-4EE3-A7D2-B83C75A5FA01}"/>
             </c:ext>
@@ -2414,11 +2986,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="677510976"/>
-        <c:axId val="677500896"/>
+        <c:axId val="-1501962144"/>
+        <c:axId val="-1501959424"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="677510976"/>
+        <c:axId val="-1501962144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="3"/>
@@ -2462,12 +3034,12 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="677500896"/>
+        <c:crossAx val="-1501959424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="677500896"/>
+        <c:axId val="-1501959424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="3"/>
@@ -2511,7 +3083,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="677510976"/>
+        <c:crossAx val="-1501962144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2525,14 +3097,14 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -2567,8 +3139,8 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="pt-BR"/>
   <c:roundedCorners val="0"/>
@@ -3515,7 +4087,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-97C3-44AA-BCC5-372EF6E9859B}"/>
             </c:ext>
@@ -4419,7 +4991,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-97C3-44AA-BCC5-372EF6E9859B}"/>
             </c:ext>
@@ -4434,11 +5006,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="677512416"/>
-        <c:axId val="677490336"/>
+        <c:axId val="-1501956704"/>
+        <c:axId val="-1501954528"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="677512416"/>
+        <c:axId val="-1501956704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4480,7 +5052,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="677490336"/>
+        <c:crossAx val="-1501954528"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4488,7 +5060,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="677490336"/>
+        <c:axId val="-1501954528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4539,7 +5111,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="677512416"/>
+        <c:crossAx val="-1501956704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4584,14 +5156,14 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -4786,7 +5358,1093 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5302,7 +6960,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5818,7 +7476,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -6334,7 +7992,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -6854,6 +8512,71 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>592667</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>94191</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1682750</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>170391</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1682748</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>94190</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1291165</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>31749</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Gráfico 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>485774</xdr:colOff>
       <xdr:row>1</xdr:row>
@@ -6870,7 +8593,7 @@
         <xdr:cNvPr id="3" name="Gráfico 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{06E7F740-EDC3-DBCC-57B6-1140A35EF69F}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{06E7F740-EDC3-DBCC-57B6-1140A35EF69F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6906,7 +8629,7 @@
         <xdr:cNvPr id="4" name="Gráfico 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CF9213AD-C576-BF3A-0F94-94BCDF986BA7}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CF9213AD-C576-BF3A-0F94-94BCDF986BA7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6942,7 +8665,7 @@
         <xdr:cNvPr id="5" name="Gráfico 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F37DC8FF-CCEB-1100-DAE8-1E7F647140CD}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F37DC8FF-CCEB-1100-DAE8-1E7F647140CD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6963,7 +8686,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -6983,7 +8706,7 @@
         <xdr:cNvPr id="2" name="Gráfico 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B1863C5-A76E-AF96-D5B3-53C7DB8788D1}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B1863C5-A76E-AF96-D5B3-53C7DB8788D1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7005,23 +8728,23 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="somas_irradiacao_dia_juliano" connectionId="1" xr16:uid="{00000000-0016-0000-0000-000001000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="somas_irradiacao_dia_juliano_1" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="somas_irradiacao_dia_juliano_1" connectionId="5" xr16:uid="{00000000-0016-0000-0000-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="somas_irradiacao_dia_juliano" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="somas_irradiacao_dia_juliano" connectionId="3" xr16:uid="{00000000-0016-0000-0100-000002000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="somas_irradiacao_dia_juliano_2" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="somas_irradiacao_dia_juliano_2" connectionId="4" xr16:uid="{00000000-0016-0000-0100-000004000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="somas_irradiacao_dia_juliano_1" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="somas_irradiacao_dia_juliano_1" connectionId="2" xr16:uid="{00000000-0016-0000-0100-000003000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="somas_irradiacao_dia_juliano" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7286,11 +9009,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00DE381F-A64E-4A77-B761-4733C6AC8E04}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7311,25 +9034,25 @@
       <c r="A1" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="G1" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="H1" s="17" t="s">
+      <c r="H1" s="16" t="s">
         <v>28</v>
       </c>
       <c r="I1" t="s">
@@ -7365,19 +9088,19 @@
         <f>B2/1</f>
         <v>183.04757086666655</v>
       </c>
-      <c r="G2" s="16">
+      <c r="G2" s="19">
         <f>D2/($B$21*(24*31))</f>
         <v>0.18881399454341194</v>
       </c>
-      <c r="H2" s="16">
+      <c r="H2" s="15">
         <f>E2/F2</f>
         <v>0.76743772821013623</v>
       </c>
       <c r="I2">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="J2">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -7406,19 +9129,19 @@
         <f t="shared" ref="F3:F13" si="2">B3/1</f>
         <v>171.43549084923526</v>
       </c>
-      <c r="G3" s="16">
+      <c r="G3" s="19">
         <f>D3/($B$21*(24*30))</f>
         <v>0.18717918344784013</v>
       </c>
-      <c r="H3" s="16">
+      <c r="H3" s="15">
         <f t="shared" ref="H3:H13" si="3">E3/F3</f>
         <v>0.78612084005968286</v>
       </c>
       <c r="I3">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="J3">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -7447,19 +9170,19 @@
         <f t="shared" si="2"/>
         <v>188.82980785481257</v>
       </c>
-      <c r="G4" s="16">
+      <c r="G4" s="19">
         <f t="shared" ref="G4:G11" si="4">D4/($B$21*(24*31))</f>
         <v>0.1946469648684381</v>
       </c>
-      <c r="H4" s="16">
+      <c r="H4" s="15">
         <f t="shared" si="3"/>
         <v>0.76691992385791696</v>
       </c>
       <c r="I4">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="J4">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="K4">
         <v>0</v>
@@ -7488,22 +9211,22 @@
         <f t="shared" si="2"/>
         <v>186.30746214999982</v>
       </c>
-      <c r="G5" s="16">
+      <c r="G5" s="19">
         <f t="shared" si="4"/>
         <v>0.16706979694461638</v>
       </c>
-      <c r="H5" s="16">
+      <c r="H5" s="15">
         <f t="shared" si="3"/>
         <v>0.66717633041836111</v>
       </c>
       <c r="I5">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="J5">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="K5">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -7529,22 +9252,22 @@
         <f t="shared" si="2"/>
         <v>150.25488893333323</v>
       </c>
-      <c r="G6" s="16">
+      <c r="G6" s="19">
         <f>D6/($B$21*(24*28))</f>
         <v>0.17039589467627844</v>
       </c>
-      <c r="H6" s="16">
+      <c r="H6" s="15">
         <f t="shared" si="3"/>
         <v>0.76207863874076298</v>
       </c>
       <c r="I6">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="J6">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="K6">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -7570,19 +9293,19 @@
         <f t="shared" si="2"/>
         <v>161.74506135833323</v>
       </c>
-      <c r="G7" s="16">
+      <c r="G7" s="19">
         <f>D7/($B$21*(24*31))</f>
         <v>0.17197996194144483</v>
       </c>
-      <c r="H7" s="16">
+      <c r="H7" s="15">
         <f t="shared" si="3"/>
         <v>0.79107881631677845</v>
       </c>
       <c r="I7">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="J7">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="K7">
         <v>0</v>
@@ -7611,19 +9334,13 @@
         <f t="shared" si="2"/>
         <v>154.26365726666654</v>
       </c>
-      <c r="G8" s="16">
+      <c r="G8" s="19">
         <f>D8/($B$21*(24*30))</f>
         <v>0.14522624970386161</v>
       </c>
-      <c r="H8" s="16">
+      <c r="H8" s="15">
         <f t="shared" si="3"/>
         <v>0.67781940114403372</v>
-      </c>
-      <c r="I8">
-        <v>14</v>
-      </c>
-      <c r="J8">
-        <v>17</v>
       </c>
       <c r="K8">
         <v>0</v>
@@ -7652,11 +9369,11 @@
         <f t="shared" si="2"/>
         <v>146.36008349166653</v>
       </c>
-      <c r="G9" s="16">
+      <c r="G9" s="19">
         <f>D9/($B$21*(24*31))</f>
         <v>2.9552697342779186E-2</v>
       </c>
-      <c r="H9" s="16">
+      <c r="H9" s="15">
         <f t="shared" si="3"/>
         <v>0.15022679885448156</v>
       </c>
@@ -7664,10 +9381,10 @@
         <v>0</v>
       </c>
       <c r="J9">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="K9">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -7693,22 +9410,22 @@
         <f t="shared" si="2"/>
         <v>119.29126767499992</v>
       </c>
-      <c r="G10" s="16">
+      <c r="G10" s="19">
         <f>D10/($B$21*(24*30))</f>
         <v>0.12738687514806915</v>
       </c>
-      <c r="H10" s="16">
+      <c r="H10" s="15">
         <f t="shared" si="3"/>
         <v>0.76886223018846678</v>
       </c>
       <c r="I10">
+        <v>3</v>
+      </c>
+      <c r="J10">
+        <v>27</v>
+      </c>
+      <c r="K10">
         <v>0</v>
-      </c>
-      <c r="J10">
-        <v>6</v>
-      </c>
-      <c r="K10">
-        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -7734,19 +9451,19 @@
         <f t="shared" si="2"/>
         <v>137.0277508499999</v>
       </c>
-      <c r="G11" s="16">
+      <c r="G11" s="19">
         <f t="shared" si="4"/>
         <v>0.15594263704518879</v>
       </c>
-      <c r="H11" s="16">
+      <c r="H11" s="15">
         <f t="shared" si="3"/>
         <v>0.84669945497846966</v>
       </c>
       <c r="I11">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="J11">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K11">
         <v>0</v>
@@ -7775,11 +9492,11 @@
         <f t="shared" si="2"/>
         <v>155.30792533333326</v>
       </c>
-      <c r="G12" s="16">
+      <c r="G12" s="19">
         <f>D12/($B$21*(24*31))</f>
         <v>0.16724939052815796</v>
       </c>
-      <c r="H12" s="16">
+      <c r="H12" s="15">
         <f t="shared" si="3"/>
         <v>0.80120538785049844</v>
       </c>
@@ -7807,11 +9524,11 @@
         <f t="shared" si="2"/>
         <v>152.29600091666654</v>
       </c>
-      <c r="G13" s="16">
+      <c r="G13" s="19">
         <f>D13/($B$21*(24*30))</f>
         <v>9.5257837795151221E-2</v>
       </c>
-      <c r="H13" s="16">
+      <c r="H13" s="15">
         <f t="shared" si="3"/>
         <v>0.45034434784691174</v>
       </c>
@@ -7827,10 +9544,10 @@
         <f>335/1000</f>
         <v>0.33500000000000002</v>
       </c>
-      <c r="C15" s="15" t="s">
+      <c r="C15" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="D15" s="15"/>
+      <c r="D15" s="18"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
@@ -7915,14 +9632,15 @@
     <mergeCell ref="C15:D15"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H96"/>
   <sheetViews>
-    <sheetView topLeftCell="A65" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -10288,7 +12006,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H366"/>
   <sheetViews>
     <sheetView topLeftCell="A284" workbookViewId="0">

</xml_diff>